<commit_message>
Avance en exportar excel
</commit_message>
<xml_diff>
--- a/personas.xlsx
+++ b/personas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>numero de cuenta</t>
   </si>
@@ -26,6 +26,10 @@
   </si>
   <si>
     <t>apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1224100619Dariel</t>
   </si>
 </sst>
 </file>
@@ -357,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,6 +381,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>